<commit_message>
Add in using the characteristic sheet and fix issue
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/full_4.xlsx
+++ b/tests/integration_test_files/full_4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C83426-63BF-734D-8D6D-6739DF1B078C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46FACDCA-5517-F845-9590-917B998171DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31360" yWindow="2460" windowWidth="58900" windowHeight="23540" firstSheet="7" activeTab="15" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="30120" yWindow="500" windowWidth="58640" windowHeight="23700" firstSheet="4" activeTab="16" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -29,14 +29,15 @@
     <sheet name="studyDesignInterventions" sheetId="25" r:id="rId14"/>
     <sheet name="studyDesignIndications" sheetId="6" r:id="rId15"/>
     <sheet name="studyDesignPopulations" sheetId="7" r:id="rId16"/>
-    <sheet name="studyDesignOE" sheetId="8" r:id="rId17"/>
-    <sheet name="studyDesignEstimands" sheetId="9" r:id="rId18"/>
-    <sheet name="studyDesignProcedures" sheetId="11" r:id="rId19"/>
-    <sheet name="studyDesignEncounters" sheetId="12" r:id="rId20"/>
-    <sheet name="studyDesignElements" sheetId="13" r:id="rId21"/>
-    <sheet name="dictionaries" sheetId="20" r:id="rId22"/>
-    <sheet name="studyDesignContent" sheetId="16" r:id="rId23"/>
-    <sheet name="configuration" sheetId="10" r:id="rId24"/>
+    <sheet name="studyDesignCharacteristics" sheetId="26" r:id="rId17"/>
+    <sheet name="studyDesignOE" sheetId="8" r:id="rId18"/>
+    <sheet name="studyDesignEstimands" sheetId="9" r:id="rId19"/>
+    <sheet name="studyDesignProcedures" sheetId="11" r:id="rId20"/>
+    <sheet name="studyDesignEncounters" sheetId="12" r:id="rId21"/>
+    <sheet name="studyDesignElements" sheetId="13" r:id="rId22"/>
+    <sheet name="dictionaries" sheetId="20" r:id="rId23"/>
+    <sheet name="studyDesignContent" sheetId="16" r:id="rId24"/>
+    <sheet name="configuration" sheetId="10" r:id="rId25"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1813" uniqueCount="826">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1829" uniqueCount="833">
   <si>
     <t>Screening</t>
   </si>
@@ -2560,6 +2561,27 @@
   </si>
   <si>
     <t>FEMALE</t>
+  </si>
+  <si>
+    <t>characteristics</t>
+  </si>
+  <si>
+    <t>CHAR1</t>
+  </si>
+  <si>
+    <t>Male subjects</t>
+  </si>
+  <si>
+    <t>Subject is male</t>
+  </si>
+  <si>
+    <t>Female subjects</t>
+  </si>
+  <si>
+    <t>Subject is female</t>
+  </si>
+  <si>
+    <t>CHAR2</t>
   </si>
 </sst>
 </file>
@@ -5282,10 +5304,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A8C2F56-38DA-1440-8447-6C36029D01F5}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5298,9 +5320,10 @@
     <col min="6" max="6" width="26.6640625" customWidth="1"/>
     <col min="7" max="7" width="19.1640625" customWidth="1"/>
     <col min="8" max="8" width="22.33203125" customWidth="1"/>
+    <col min="9" max="9" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
         <v>796</v>
       </c>
@@ -5325,8 +5348,11 @@
       <c r="H1" s="22" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I1" s="22" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>799</v>
       </c>
@@ -5347,7 +5373,7 @@
       </c>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>821</v>
       </c>
@@ -5363,8 +5389,11 @@
       <c r="H3" s="3" t="s">
         <v>824</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I3" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>821</v>
       </c>
@@ -5379,6 +5408,9 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3" t="s">
         <v>825</v>
+      </c>
+      <c r="I4" t="s">
+        <v>832</v>
       </c>
     </row>
   </sheetData>
@@ -5388,11 +5420,77 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F468BB1-BDAF-ED4A-934C-1B86ABB62DE9}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="38" t="s">
+        <v>220</v>
+      </c>
+      <c r="B1" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="38" t="s">
+        <v>495</v>
+      </c>
+      <c r="D1" s="38" t="s">
+        <v>222</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
+        <v>827</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>828</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>828</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="15" t="s">
+        <v>832</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>830</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>830</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>831</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9162AE3F-0A5D-824F-8BC1-E6A493EFAA49}">
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E7"/>
+      <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5799,7 +5897,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D036654E-7FF8-D440-BC0A-D74BC57BB3C9}">
   <dimension ref="A1:H1"/>
   <sheetViews>
@@ -5841,97 +5939,6 @@
       </c>
       <c r="H1" s="12" t="s">
         <v>48</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B29E6393-3A18-464C-A40D-B41879707264}">
-  <dimension ref="A1:G4"/>
-  <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" customWidth="1"/>
-    <col min="4" max="4" width="14.83203125" customWidth="1"/>
-    <col min="5" max="5" width="50.33203125" style="31" customWidth="1"/>
-    <col min="6" max="6" width="24" style="20" customWidth="1"/>
-    <col min="7" max="7" width="29.6640625" customWidth="1"/>
-    <col min="8" max="8" width="14.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>495</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="E1" s="33" t="s">
-        <v>86</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>193</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>193</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>193</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="14"/>
-    </row>
-    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>741</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>738</v>
-      </c>
-      <c r="E3" s="31" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>742</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>739</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="31" t="s">
-        <v>737</v>
       </c>
     </row>
   </sheetData>
@@ -6004,6 +6011,97 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B29E6393-3A18-464C-A40D-B41879707264}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" customWidth="1"/>
+    <col min="5" max="5" width="50.33203125" style="31" customWidth="1"/>
+    <col min="6" max="6" width="24" style="20" customWidth="1"/>
+    <col min="7" max="7" width="29.6640625" customWidth="1"/>
+    <col min="8" max="8" width="14.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>495</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="14"/>
+    </row>
+    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>741</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>738</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>742</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>739</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="31" t="s">
+        <v>737</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CB4E9D5-B601-284A-9651-0AA604C2B9D1}">
   <dimension ref="A1:H13"/>
   <sheetViews>
@@ -6314,7 +6412,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6FA5DC6-70BE-E845-A085-20526138A835}">
   <dimension ref="A1:E8"/>
   <sheetViews>
@@ -6458,7 +6556,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{989384DC-1C54-514A-8A1E-ADD84D891BA4}">
   <dimension ref="A1:G5"/>
   <sheetViews>
@@ -6578,7 +6676,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2976DC75-5A85-2A48-9FBD-A6539815E624}">
   <dimension ref="A1:D139"/>
   <sheetViews>
@@ -7852,7 +7950,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED6534B-B4C9-924A-BB14-180C2C37C6F1}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -8228,7 +8326,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Initial code and test
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/full_4.xlsx
+++ b/tests/integration_test_files/full_4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46FACDCA-5517-F845-9590-917B998171DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2FFAD8D-0299-5645-967B-4E02E2E78E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30120" yWindow="500" windowWidth="58640" windowHeight="23700" firstSheet="4" activeTab="16" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="30120" yWindow="500" windowWidth="58640" windowHeight="23700" firstSheet="7" activeTab="23" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1829" uniqueCount="833">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1830" uniqueCount="834">
   <si>
     <t>Screening</t>
   </si>
@@ -2582,6 +2582,9 @@
   </si>
   <si>
     <t>CHAR2</t>
+  </si>
+  <si>
+    <t>&lt;usdm:macro id="bc" name="Systolic blood pressure" activity="Vital signs / Temperature"&gt;</t>
   </si>
 </sst>
 </file>
@@ -2823,10 +2826,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3809,7 +3812,7 @@
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5423,7 +5426,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F468BB1-BDAF-ED4A-934C-1B86ABB62DE9}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -6680,8 +6683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2976DC75-5A85-2A48-9FBD-A6539815E624}">
   <dimension ref="A1:D139"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6812,8 +6815,11 @@
       <c r="C13" s="6" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="D13" s="6" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>243</v>
       </c>
@@ -8099,120 +8105,120 @@
       <c r="A1" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="51" t="s">
         <v>120</v>
       </c>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="51" t="s">
         <v>122</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
     </row>
     <row r="3" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="52" t="s">
         <v>806</v>
       </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
     </row>
     <row r="4" spans="1:6" ht="98" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="52" t="s">
         <v>124</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
       <c r="F4" s="16"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="51" t="s">
         <v>129</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
       <c r="F5" s="14"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="51" t="s">
         <v>130</v>
       </c>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
       <c r="F6" s="14"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="52" t="s">
         <v>678</v>
       </c>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
       <c r="F7" s="14"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="52" t="s">
+      <c r="B8" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
       <c r="F8" s="14"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="52" t="s">
+      <c r="B9" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="C9" s="52"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
       <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="52" t="s">
         <v>707</v>
       </c>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
       <c r="F10" s="14"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -8304,16 +8310,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8656,8 +8662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136502A0-3DDE-CC47-9DA7-EB2F3073B24B}">
   <dimension ref="A1:V68"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24:C25"/>
+    <sheetView topLeftCell="A13" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11945,17 +11951,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="98eacbea-7562-4a40-a7f2-e999cdc0cec5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="75bf9804-c18d-470a-a27f-eeaf4abcd247" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D47D794EB48E7144959FE534A5ED3D9A" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e2a26abefe6b107b571df4f2e43af2ce">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="98eacbea-7562-4a40-a7f2-e999cdc0cec5" xmlns:ns3="75bf9804-c18d-470a-a27f-eeaf4abcd247" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5806404ce956f9af473b927dc8d5ee33" ns2:_="" ns3:_="">
     <xsd:import namespace="98eacbea-7562-4a40-a7f2-e999cdc0cec5"/>
@@ -12156,6 +12151,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="98eacbea-7562-4a40-a7f2-e999cdc0cec5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="75bf9804-c18d-470a-a27f-eeaf4abcd247" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0D2739C-381D-470B-B6E1-B86FD5C25B2E}">
   <ds:schemaRefs>
@@ -12165,23 +12171,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AE94761-8578-4804-B593-FBFFCD1EC013}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="98eacbea-7562-4a40-a7f2-e999cdc0cec5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="75bf9804-c18d-470a-a27f-eeaf4abcd247"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028E3775-7751-44E5-835D-F091B807F690}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12198,4 +12187,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AE94761-8578-4804-B593-FBFFCD1EC013}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="98eacbea-7562-4a40-a7f2-e999cdc0cec5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="75bf9804-c18d-470a-a27f-eeaf4abcd247"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add BC macro and tests
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/full_4.xlsx
+++ b/tests/integration_test_files/full_4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2FFAD8D-0299-5645-967B-4E02E2E78E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6422C079-B505-C947-8369-30DF8114C99D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30120" yWindow="500" windowWidth="58640" windowHeight="23700" firstSheet="7" activeTab="23" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
@@ -2584,7 +2584,7 @@
     <t>CHAR2</t>
   </si>
   <si>
-    <t>&lt;usdm:macro id="bc" name="Systolic blood pressure" activity="Vital signs / Temperature"&gt;</t>
+    <t>&lt;usdm:macro id="bc" name="Body temperature" activity="Vital signs / Temperature"&gt;</t>
   </si>
 </sst>
 </file>
@@ -6684,7 +6684,7 @@
   <dimension ref="A1:D139"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8663,7 +8663,7 @@
   <dimension ref="A1:V68"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>